<commit_message>
Changes Tim has made
Modification includes the first part “Research question”…My battery is
drying soon, I will continue the other part during the weekend.
</commit_message>
<xml_diff>
--- a/Project timeline.xlsx
+++ b/Project timeline.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TimKuo/Documents/TheGreatGrapeProblem/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19140" windowHeight="7840"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Expose</t>
   </si>
@@ -64,13 +74,22 @@
   </si>
   <si>
     <t>Project Presentation</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,12 +98,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -101,7 +130,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,24 +138,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,7 +229,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,7 +264,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -428,146 +473,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M18"/>
+  <dimension ref="B1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.81640625" customWidth="1"/>
-    <col min="3" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" style="1" customWidth="1"/>
+    <col min="3" max="13" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="C1" t="s">
+    <row r="1" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="C2" s="1">
+    <row r="2" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="7">
         <v>42835</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="7">
         <v>42842</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E3" s="7">
         <v>42849</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F3" s="7">
         <v>42856</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G3" s="7">
         <v>42863</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H3" s="7">
         <v>42870</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I3" s="7">
         <v>42877</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J3" s="7">
         <v>42884</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K3" s="7">
         <v>42891</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L3" s="7">
         <v>42898</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M3" s="7">
         <v>42905</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B4" s="4" t="s">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B5" s="2" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B9" s="5" t="s">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B10" s="2" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B11" s="5" t="s">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B12" s="2" t="s">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B13" s="6" t="s">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B14" s="6" t="s">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B15" s="6" t="s">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B16" s="6" t="s">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B17" s="5" t="s">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B18" s="4" t="s">
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M18" s="3"/>
+      <c r="M19" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:M2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -579,7 +650,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -591,7 +662,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revised Intro, Methods and Timeline
I’ve made things more compact, as well as copy the timeline table here.
I think we will need 2 pages to contain everything ;-)
</commit_message>
<xml_diff>
--- a/Project timeline.xlsx
+++ b/Project timeline.xlsx
@@ -31,45 +31,15 @@
     <t>Expose</t>
   </si>
   <si>
-    <t>Prepare research question</t>
-  </si>
-  <si>
     <t>START DATE</t>
   </si>
   <si>
     <t>Model the system</t>
   </si>
   <si>
-    <t>UML-diagrams</t>
-  </si>
-  <si>
-    <t>Research State of the art</t>
-  </si>
-  <si>
-    <t>Project structure</t>
-  </si>
-  <si>
-    <t>Project timeline</t>
-  </si>
-  <si>
     <t>Implementation</t>
   </si>
   <si>
-    <t>Set up platform</t>
-  </si>
-  <si>
-    <t>Implement the world</t>
-  </si>
-  <si>
-    <t>Implement a single car</t>
-  </si>
-  <si>
-    <t>Test run</t>
-  </si>
-  <si>
-    <t>Expand the population</t>
-  </si>
-  <si>
     <t>Project Report</t>
   </si>
   <si>
@@ -83,12 +53,45 @@
   </si>
   <si>
     <t>June</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Prepare research question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Project timeline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Research State of the art</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Project structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    UML-diagrams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Set up platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Implement the world</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Implement a single car</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Test run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Expand the population</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="m/d;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,15 +108,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Garamond"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Garamond"/>
     </font>
   </fonts>
   <fills count="3">
@@ -130,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -153,25 +156,149 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,171 +600,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M19"/>
+  <dimension ref="B1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.83203125" style="1" customWidth="1"/>
-    <col min="3" max="13" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="13" width="8.33203125" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4"/>
+      <c r="C3" s="19">
+        <v>42835</v>
+      </c>
+      <c r="D3" s="19">
+        <v>42842</v>
+      </c>
+      <c r="E3" s="19">
+        <v>42849</v>
+      </c>
+      <c r="F3" s="19">
+        <v>42856</v>
+      </c>
+      <c r="G3" s="19">
+        <v>42863</v>
+      </c>
+      <c r="H3" s="19">
+        <v>42870</v>
+      </c>
+      <c r="I3" s="19">
+        <v>42877</v>
+      </c>
+      <c r="J3" s="19">
+        <v>42884</v>
+      </c>
+      <c r="K3" s="19">
+        <v>42891</v>
+      </c>
+      <c r="L3" s="19">
+        <v>42898</v>
+      </c>
+      <c r="M3" s="19">
+        <v>42905</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="13"/>
+    </row>
+    <row r="6" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="13"/>
+    </row>
+    <row r="7" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="13"/>
+    </row>
+    <row r="9" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="6" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="13"/>
+    </row>
+    <row r="10" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="13"/>
+    </row>
+    <row r="11" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="13"/>
+    </row>
+    <row r="12" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="13"/>
+    </row>
+    <row r="13" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="13"/>
+    </row>
+    <row r="14" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="13"/>
+    </row>
+    <row r="15" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="13"/>
+    </row>
+    <row r="16" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="7">
-        <v>42835</v>
-      </c>
-      <c r="D3" s="7">
-        <v>42842</v>
-      </c>
-      <c r="E3" s="7">
-        <v>42849</v>
-      </c>
-      <c r="F3" s="7">
-        <v>42856</v>
-      </c>
-      <c r="G3" s="7">
-        <v>42863</v>
-      </c>
-      <c r="H3" s="7">
-        <v>42870</v>
-      </c>
-      <c r="I3" s="7">
-        <v>42877</v>
-      </c>
-      <c r="J3" s="7">
-        <v>42884</v>
-      </c>
-      <c r="K3" s="7">
-        <v>42891</v>
-      </c>
-      <c r="L3" s="7">
-        <v>42898</v>
-      </c>
-      <c r="M3" s="7">
-        <v>42905</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="13"/>
+    </row>
+    <row r="17" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="13"/>
+    </row>
+    <row r="18" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M19" s="2"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:M2"/>
+    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>